<commit_message>
added fresh data for registration
</commit_message>
<xml_diff>
--- a/src/main/java/com/ecom/qa/testdata/TestData.xlsx
+++ b/src/main/java/com/ecom/qa/testdata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10170" windowHeight="3555"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="5955"/>
   </bookViews>
   <sheets>
     <sheet name="RegDetails" sheetId="1" r:id="rId1"/>
@@ -52,33 +52,9 @@
     <t>Status</t>
   </si>
   <si>
-    <t>bat</t>
-  </si>
-  <si>
-    <t>ujay</t>
-  </si>
-  <si>
     <t>Vir</t>
   </si>
   <si>
-    <t>Jay</t>
-  </si>
-  <si>
-    <t>Ney</t>
-  </si>
-  <si>
-    <t>Punde</t>
-  </si>
-  <si>
-    <t>Yaty</t>
-  </si>
-  <si>
-    <t>vir</t>
-  </si>
-  <si>
-    <t>Singh</t>
-  </si>
-  <si>
     <t>Neui</t>
   </si>
   <si>
@@ -88,16 +64,40 @@
     <t>Yuki</t>
   </si>
   <si>
-    <t>a20@email.com</t>
-  </si>
-  <si>
-    <t>a21@email.com</t>
-  </si>
-  <si>
-    <t>a22@email.com</t>
-  </si>
-  <si>
-    <t>a23@email.com</t>
+    <t>a25@email.com</t>
+  </si>
+  <si>
+    <t>a26@email.com</t>
+  </si>
+  <si>
+    <t>a27@email.com</t>
+  </si>
+  <si>
+    <t>a28@email.com</t>
+  </si>
+  <si>
+    <t>Ronald</t>
+  </si>
+  <si>
+    <t>Delver</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Con</t>
+  </si>
+  <si>
+    <t>Asult</t>
+  </si>
+  <si>
+    <t>Bolswa</t>
+  </si>
+  <si>
+    <t>Jimmy</t>
+  </si>
+  <si>
+    <t>Lever</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,16 +505,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
@@ -522,16 +522,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -539,16 +539,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -556,16 +556,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
adding changes made to page classes
</commit_message>
<xml_diff>
--- a/src/main/java/com/ecom/qa/testdata/TestData.xlsx
+++ b/src/main/java/com/ecom/qa/testdata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="7245"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11505" windowHeight="4110"/>
   </bookViews>
   <sheets>
     <sheet name="RegDetails" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <calcPr calcId="0"/>
   <oleSize ref="A1"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>FirstName</t>
   </si>
@@ -52,72 +52,59 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Delverrw</t>
-  </si>
-  <si>
-    <t>Coner</t>
-  </si>
-  <si>
-    <t>Bolswarv</t>
-  </si>
-  <si>
-    <t>Leverrj</t>
-  </si>
-  <si>
-    <t>eNeuiteq</t>
-  </si>
-  <si>
-    <t>dZuranewd</t>
-  </si>
-  <si>
-    <t>qVirweq</t>
-  </si>
-  <si>
-    <t>gYukirrdde</t>
-  </si>
-  <si>
-    <t>Ronaldyqwqa</t>
-  </si>
-  <si>
-    <t>Petereshd</t>
-  </si>
-  <si>
-    <t>Asultrfme</t>
-  </si>
-  <si>
-    <t>Jimmypykq</t>
-  </si>
-  <si>
-    <t>a107@email.com</t>
-  </si>
-  <si>
-    <t>a108@email.com</t>
-  </si>
-  <si>
-    <t>a109@email.com</t>
-  </si>
-  <si>
-    <t>a110@email.com</t>
-  </si>
-  <si>
-    <t>Registration successful for eNeuiteq</t>
-  </si>
-  <si>
-    <t>Registration successful for dZuranewd</t>
-  </si>
-  <si>
-    <t>Registration successful for qVirweq</t>
-  </si>
-  <si>
-    <t>Registration successful for gYukirrdde</t>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Ron</t>
+  </si>
+  <si>
+    <t>Jin</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>Kio</t>
+  </si>
+  <si>
+    <t>Conery</t>
+  </si>
+  <si>
+    <t>Butna</t>
+  </si>
+  <si>
+    <t>Amy</t>
+  </si>
+  <si>
+    <t>Swan</t>
+  </si>
+  <si>
+    <t>Jen</t>
+  </si>
+  <si>
+    <t>Loper</t>
+  </si>
+  <si>
+    <t>Kou</t>
+  </si>
+  <si>
+    <t>a120@email.com</t>
+  </si>
+  <si>
+    <t>a121@email.com</t>
+  </si>
+  <si>
+    <t>a122@email.com</t>
+  </si>
+  <si>
+    <t>a123@email.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,17 +470,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="59.85546875" collapsed="true"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="59.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -518,42 +505,36 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -561,39 +542,33 @@
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>